<commit_message>
new lasso results interpreted
</commit_message>
<xml_diff>
--- a/Graphics and Supplements/Graphics source/Coho life cycle graphic.xlsx
+++ b/Graphics and Supplements/Graphics source/Coho life cycle graphic.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire\Documents\GitHub\Fish_hydrometrics_MS\Graphics and Supplements\Graphics source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ck798\Documents\GitHub\Fish_hydrometrics_MS\Graphics and Supplements\Graphics source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0C2EF2-C955-4500-BA35-ECD4A91646A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80556E5B-1AC8-47EA-8AE9-0999EB5BE851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-73620" yWindow="1290" windowWidth="27645" windowHeight="14565" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dry season start" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Dry season start'!$A$2:$E$14</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$2:$D$16</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="46">
   <si>
     <t>d1</t>
   </si>
@@ -177,12 +179,48 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <t>During/after parents' spawning</t>
+  </si>
+  <si>
+    <t>Before parents' spawning</t>
+  </si>
+  <si>
+    <t>d1, first dry season</t>
+  </si>
+  <si>
+    <t>d2, second dry season</t>
+  </si>
+  <si>
+    <t>Dec-Mar:</t>
+  </si>
+  <si>
+    <t>Alignment of seasons and life stages experienced by a salmon cohort for two species, Scott River, CA</t>
+  </si>
+  <si>
+    <t>Abbreviated season identifier (e.g., first wet season experienced by a salmon cohort)</t>
+  </si>
+  <si>
+    <t>Life stage</t>
+  </si>
+  <si>
+    <t>Season ID</t>
+  </si>
+  <si>
+    <t>Before/during parents' spawning</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>Approx. dates</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,6 +240,38 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFEE4612"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -263,7 +333,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -395,24 +465,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -427,6 +528,88 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,165 +898,165 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.86328125" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="23.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="18" t="s">
+    <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="14" t="s">
+    <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C13" s="5" t="s">
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C14" s="14" t="s">
+    <row r="14" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -881,7 +1064,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
@@ -889,7 +1072,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
@@ -897,7 +1080,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="2" t="s">
         <v>30</v>
       </c>
@@ -913,4 +1096,245 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F91793-9033-4B47-8A3A-26D9D07B8ECE}">
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="23.46484375" customWidth="1"/>
+    <col min="3" max="3" width="19.1328125" customWidth="1"/>
+    <col min="4" max="4" width="16.53125" customWidth="1"/>
+    <col min="5" max="5" width="18.9296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="43"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="44"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="35"/>
+      <c r="B5" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="41"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="5.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="34"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="23.35" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="35"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="35"/>
+      <c r="B12" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="41"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A14" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B19" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B12:E12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>